<commit_message>
2024-05-27 Hockey Pool, Resource
</commit_message>
<xml_diff>
--- a/Python/Hockey pool/2024/My Predictions.xlsx
+++ b/Python/Hockey pool/2024/My Predictions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abrig\Documents\Coding_Practice\Python\Hockey pool\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABriggs\Documents\Coding Practice\Coding_Practice\Python\Hockey pool\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FF5445-DA12-4875-A5CF-394F6007BF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9ED06C-5720-4A08-AC87-7C6A851A79C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4830" windowWidth="15990" windowHeight="24840" xr2:uid="{7BF13B1A-4770-4E31-9A10-40459726CAB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BF13B1A-4770-4E31-9A10-40459726CAB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,30 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -47,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="137">
   <si>
     <t>NYI</t>
   </si>
@@ -1079,9 +1090,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1119,7 +1130,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1225,7 +1236,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1367,7 +1378,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1377,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0969FCB-44D6-4DD7-80C6-C6E6D39A1DF9}">
   <dimension ref="A1:BL90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AF52" sqref="AF52"/>
+    <sheetView tabSelected="1" topLeftCell="G57" workbookViewId="0">
+      <selection activeCell="M76" sqref="M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9997,8 +10008,12 @@
       <c r="K76" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
+      <c r="L76" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M76" s="3">
+        <v>45439</v>
+      </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>

</xml_diff>